<commit_message>
copy shadow map pass 추가
CopyResource의 사용이 불가능하기에 GPU를 사용하여 복사 unreal의 CopyShadowMap.usf를 사용하도록 함

렌더러에 DrawRactengle 함수 추가

렌더러에서 스크린 매쉬를 그리는 함수

그렇기에 기존에 screen mesh를 사용하던 곳을 해당 함수로 변경
</commit_message>
<xml_diff>
--- a/Library/bin/graphics/table/PipelineStateTable.xlsx
+++ b/Library/bin/graphics/table/PipelineStateTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\menew\Documents\GitHub\REngine\Library\bin\graphics\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F023D947-730F-4902-9D67-6AC95005FA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4DACBB-09B5-473E-B632-93780EE4A71C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="2115" windowWidth="25410" windowHeight="11385" activeTab="1" xr2:uid="{A66BFFD3-44BC-431C-A43B-437626919F3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A66BFFD3-44BC-431C-A43B-437626919F3E}"/>
   </bookViews>
   <sheets>
     <sheet name="PipelineState" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="141">
   <si>
     <t>../PipelineStateTable.json</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -409,10 +409,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>00000000-0000-0000-0007-000000000000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>00000000-0000-0000-0003-000000000000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -573,6 +569,30 @@
   </si>
   <si>
     <t>00000000-0000-0000-0026-000000000000</t>
+  </si>
+  <si>
+    <t>Copy2DDepth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CopyCubeDepth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Copy2DDepthPS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CopyCubeDepthPS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CopyCubeDepthGS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ScreenVS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -767,8 +787,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ACB5A5A8-FBF7-40DA-A057-A7CFFAE5E7F8}" name="표2" displayName="표2" ref="A2:G18" totalsRowShown="0">
-  <autoFilter ref="A2:G18" xr:uid="{ACB5A5A8-FBF7-40DA-A057-A7CFFAE5E7F8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ACB5A5A8-FBF7-40DA-A057-A7CFFAE5E7F8}" name="표2" displayName="표2" ref="A2:G20" totalsRowShown="0">
+  <autoFilter ref="A2:G20" xr:uid="{ACB5A5A8-FBF7-40DA-A057-A7CFFAE5E7F8}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{E179A3F3-F267-42A3-8D7C-10D95D6E7C88}" name="UUID : String"/>
     <tableColumn id="2" xr3:uid="{37C18820-78B7-454B-9AA8-AB44AD1FAFF0}" name="Vertex : String"/>
@@ -1202,10 +1222,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
         <v>66</v>
@@ -1280,10 +1300,10 @@
         <v>66</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>82</v>
@@ -1363,10 +1383,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C10" t="s">
         <v>66</v>
@@ -1386,10 +1406,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C11" t="s">
         <v>66</v>
@@ -1409,10 +1429,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C12" t="s">
         <v>66</v>
@@ -1432,10 +1452,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C13" t="s">
         <v>66</v>
@@ -1455,10 +1475,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C14" t="s">
         <v>66</v>
@@ -1478,10 +1498,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" t="s">
         <v>66</v>
@@ -1501,10 +1521,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C16" t="s">
         <v>66</v>
@@ -1524,10 +1544,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C17" t="s">
         <v>66</v>
@@ -1547,10 +1567,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C18" t="s">
         <v>66</v>
@@ -1579,10 +1599,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07EDAF6D-248C-4551-840F-371628ACD4EB}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1621,13 +1641,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
         <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1638,7 +1658,7 @@
         <v>91</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1649,7 +1669,7 @@
         <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1657,10 +1677,10 @@
         <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1668,10 +1688,10 @@
         <v>89</v>
       </c>
       <c r="B7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" t="s">
         <v>98</v>
-      </c>
-      <c r="C7" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1679,10 +1699,10 @@
         <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1690,109 +1710,134 @@
         <v>88</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" t="s">
         <v>102</v>
-      </c>
-      <c r="B10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C10" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B13" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="C13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" t="s">
         <v>120</v>
-      </c>
-      <c r="C14" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" t="s">
         <v>124</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>125</v>
-      </c>
-      <c r="C15" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" t="s">
         <v>130</v>
       </c>
-      <c r="B16" t="s">
-        <v>131</v>
-      </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" t="s">
         <v>131</v>
-      </c>
-      <c r="D17" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D18" t="s">
-        <v>133</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>136</v>
+      </c>
+      <c r="B20" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" t="s">
+        <v>138</v>
+      </c>
+      <c r="D20" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1862,7 +1907,7 @@
         <v>40</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>41</v>
@@ -1991,7 +2036,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>74</v>
@@ -2000,7 +2045,7 @@
         <v>74</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>33</v>
@@ -2041,7 +2086,7 @@
     </row>
     <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>74</v>
@@ -2062,7 +2107,7 @@
         <v>80</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>51</v>
@@ -2071,7 +2116,7 @@
         <v>51</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>81</v>
@@ -2083,7 +2128,7 @@
         <v>51</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>81</v>
@@ -2091,7 +2136,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>33</v>
@@ -2112,7 +2157,7 @@
         <v>80</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>51</v>
@@ -2124,7 +2169,7 @@
         <v>51</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>51</v>
@@ -2136,7 +2181,7 @@
         <v>51</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>